<commit_message>
looked at a couple of functions/added to the excel
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\Profiles\LinS5\r_code\janitor_function_overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C961F9E6-2D10-3B4C-9D4C-4EC4C8133E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4817A2BA-18E1-44EE-AEC1-C7F4139356F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41560" yWindow="1120" windowWidth="28040" windowHeight="17440" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
+    <workbookView xWindow="2025" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>function_name</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>presenting_worthy</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>additional_notes</t>
+  </si>
+  <si>
+    <t>deprecated, use adorn_totals</t>
   </si>
 </sst>
 </file>
@@ -519,76 +531,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BEC45-6A70-274D-AAFF-6DFC31B3AF54}">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -596,7 +628,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -604,7 +636,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -612,7 +644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -620,17 +652,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -638,7 +670,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -646,12 +678,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -659,7 +691,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -667,12 +699,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -680,12 +712,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -693,7 +725,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -701,17 +733,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -719,7 +751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -727,7 +759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -735,17 +767,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -753,7 +785,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -761,7 +793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -769,17 +801,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
went through functions and updated presenting worthy and comments columns
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\Profiles\LinS5\r_code\janitor_function_overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4817A2BA-18E1-44EE-AEC1-C7F4139356F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68877D0-C414-4485-B2C9-70D799A9EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="2070" windowWidth="21600" windowHeight="11295" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
   <si>
     <t>function_name</t>
   </si>
@@ -128,9 +128,6 @@
     <t>round_half_up</t>
   </si>
   <si>
-    <t>round_to_fraaction</t>
-  </si>
-  <si>
     <t>row_to_names</t>
   </si>
   <si>
@@ -171,6 +168,105 @@
   </si>
   <si>
     <t>deprecated, use adorn_totals</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>ways to format/amend tabyls</t>
+  </si>
+  <si>
+    <t>might be worth mentioning just b/c it always shows as a warning when you load it in? but otherwise not important b/c janitor::chisq.test only runs when applied to a two-way tabyl, otherwise just calls stats:: chisq.test</t>
+  </si>
+  <si>
+    <t>mention in conjunction to tabyl that you can convert tables to a tabyl if you want the extra formatting that comes with it if they meet the requires of a 2-way tabyl?</t>
+  </si>
+  <si>
+    <t>highlight this is used in dan's template?</t>
+  </si>
+  <si>
+    <t>used to see if column classes conflict and prevent row binding</t>
+  </si>
+  <si>
+    <t>returns TRUE or FALSE saying if the df's can successfully row bind</t>
+  </si>
+  <si>
+    <t>can handle a vector with a date and excel datetime format and successfully convert to the Date class, but is there a lubridate equivalent to this???</t>
+  </si>
+  <si>
+    <t>need to say this function though useful is deprecated (I know hannah still uses this lol), maybe we can have a list of deprecated functions toward the end and highlight that this one is?</t>
+  </si>
+  <si>
+    <t>I don't think this is useful enough</t>
+  </si>
+  <si>
+    <t>I think convert_to_date is more useful/more worth our time but could be useful building block?</t>
+  </si>
+  <si>
+    <t>companion to row_to_names</t>
+  </si>
+  <si>
+    <t>similar schtick to chisq.test</t>
+  </si>
+  <si>
+    <t>super useful for getting rows of identical values for specific variables aka mrn</t>
+  </si>
+  <si>
+    <t>looks within each column to see if there are multiple values, not sure if super helpful for our work</t>
+  </si>
+  <si>
+    <t>could list all deprecated functions on a page</t>
+  </si>
+  <si>
+    <t>no*</t>
+  </si>
+  <si>
+    <t>more generalized version of clean_makes b/c can apply it to a vector</t>
+  </si>
+  <si>
+    <t>honestly seems super specific</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>removes empty rows and cols after being read in</t>
+  </si>
+  <si>
+    <t>removes columns with one constant value, can specify whether NA's should be considered different values from a constant value</t>
+  </si>
+  <si>
+    <t>round_to_fraction</t>
+  </si>
+  <si>
+    <t>in base r round, 12.5 and 11.5 are rounded to 12; round_half_up rounds 12.5 to 13</t>
+  </si>
+  <si>
+    <t>round to nearest fraction of a specified denominator</t>
+  </si>
+  <si>
+    <t>designate row to be column name of dataframe; not sure if it's worth our time??</t>
+  </si>
+  <si>
+    <t>could be nice to have sas people be included? But we can ask sas users how much of an issue this really is</t>
+  </si>
+  <si>
+    <t>similar to round_half_up, but can specify how many digits</t>
+  </si>
+  <si>
+    <t>enforces column all has the same value, not sure how useful this would be</t>
+  </si>
+  <si>
+    <t>can create contingency tables that are relatively easy to code but are more presentable</t>
+  </si>
+  <si>
+    <t>lowkey an uglier version of gtsummary::tbl_summary</t>
+  </si>
+  <si>
+    <t>maybe worth mentioning you can strip away the tabyl-related attributes from a df?</t>
+  </si>
+  <si>
+    <t>returns 1st non-NA value from a set of vectors, not sure if it's worth our time</t>
   </si>
 </sst>
 </file>
@@ -533,282 +629,498 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BEC45-6A70-274D-AAFF-6DFC31B3AF54}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added conditional formatting for eye candy
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\Profiles\LinS5\r_code\janitor_function_overview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68877D0-C414-4485-B2C9-70D799A9EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="6_{276FF295-ADE3-B44E-A747-B6CF3BAA8E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07A9AC87-13BB-D845-ACCE-B55251E26824}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
+    <workbookView xWindow="5400" yWindow="3200" windowWidth="26100" windowHeight="16680" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,68 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -629,18 +690,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BEC45-6A70-274D-AAFF-6DFC31B3AF54}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.09765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +715,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -665,7 +726,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -676,7 +737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -687,7 +748,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -698,7 +759,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -709,7 +770,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -720,7 +781,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -731,7 +792,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -742,7 +803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -753,7 +814,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -764,7 +825,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -778,7 +839,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -792,7 +853,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -806,7 +867,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -820,7 +881,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -831,7 +892,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -842,7 +903,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -856,7 +917,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -870,7 +931,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -881,7 +942,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -895,7 +956,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -909,7 +970,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -920,7 +981,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -934,7 +995,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -945,7 +1006,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -959,7 +1020,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -973,7 +1034,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -984,7 +1045,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -995,7 +1056,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1009,7 +1070,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1023,7 +1084,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1037,7 +1098,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1048,7 +1109,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1059,7 +1120,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1073,7 +1134,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1087,7 +1148,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1101,7 +1162,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1112,7 +1173,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1124,6 +1185,17 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"maybe"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added some caroline notes
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="6_{276FF295-ADE3-B44E-A747-B6CF3BAA8E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07A9AC87-13BB-D845-ACCE-B55251E26824}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="6_{276FF295-ADE3-B44E-A747-B6CF3BAA8E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{445451C4-21B9-1546-BF04-0F268DB573A8}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="3200" windowWidth="26100" windowHeight="16680" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
   <si>
     <t>function_name</t>
   </si>
@@ -267,6 +267,51 @@
   </si>
   <si>
     <t>returns 1st non-NA value from a set of vectors, not sure if it's worth our time</t>
+  </si>
+  <si>
+    <t>definitely</t>
+  </si>
+  <si>
+    <t>maybe I'm crazy but I feel like I would just try binding and hope for the best/take care of any errors if they pop up?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i think lubridates doesn't handle excel dates specifically: https://lubridate.tidyverse.org/reference/as_date.html </t>
+  </si>
+  <si>
+    <t>agreed -- maybe we can suggest the dplyr alternative? https://dplyr.tidyverse.org/reference/na_if.html</t>
+  </si>
+  <si>
+    <t>this is lame… how is this diff from class()??</t>
+  </si>
+  <si>
+    <t>we should check if this is burried in convert_to_date</t>
+  </si>
+  <si>
+    <t>meh, im not convinced its big enough to highlight</t>
+  </si>
+  <si>
+    <t>I think we could cut</t>
+  </si>
+  <si>
+    <t>funnily enough, ive used this LOL - but while also using make_clean_names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I didn't know base R did it this way and now I'm weirded out…. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I feel like I go through this also with matrices… </t>
+  </si>
+  <si>
+    <t>agree we ask the SAS users</t>
+  </si>
+  <si>
+    <t>I feel like I need to play around with this to understand what's going on</t>
+  </si>
+  <si>
+    <t>may as well throw it in if we are talking about what we can do with tabyls</t>
+  </si>
+  <si>
+    <t>DEPRECATED - says to use dplyr::coalesce() instead</t>
   </si>
 </sst>
 </file>
@@ -310,44 +355,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -370,11 +391,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -389,6 +410,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -688,20 +713,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BEC45-6A70-274D-AAFF-6DFC31B3AF54}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="49.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="44.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,121 +737,124 @@
       <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -835,11 +864,14 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -849,11 +881,14 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -863,11 +898,11 @@
       <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -877,33 +912,42 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
         <v>41</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -913,11 +957,14 @@
       <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -927,22 +974,22 @@
       <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -952,11 +999,11 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -966,22 +1013,25 @@
       <c r="C22" t="s">
         <v>44</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -991,22 +1041,25 @@
       <c r="C24" t="s">
         <v>39</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1016,11 +1069,11 @@
       <c r="C26" t="s">
         <v>39</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1030,33 +1083,33 @@
       <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1066,11 +1119,14 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1080,11 +1136,11 @@
       <c r="C31" t="s">
         <v>39</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1094,33 +1150,39 @@
       <c r="C32" t="s">
         <v>44</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
         <v>44</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1130,11 +1192,14 @@
       <c r="C35" t="s">
         <v>44</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1144,11 +1209,11 @@
       <c r="C36" t="s">
         <v>39</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1158,42 +1223,48 @@
       <c r="C37" t="s">
         <v>41</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
         <v>44</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="3" t="s">
         <v>76</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"yes"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"maybe"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"maybe"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated excel with final function decisions and additional information on which dataset to use
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\Profiles\LinS5\r_code\janitor_function_overview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="6_{276FF295-ADE3-B44E-A747-B6CF3BAA8E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{445451C4-21B9-1546-BF04-0F268DB573A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88687610-5403-4888-9F40-8DF9F52D5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="3200" windowWidth="26100" windowHeight="16680" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="janitor_functions" sheetId="1" r:id="rId1"/>
+    <sheet name="datasets" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">janitor_functions!$D$1:$D$39</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="107">
   <si>
     <t>function_name</t>
   </si>
@@ -158,15 +162,9 @@
     <t>yes</t>
   </si>
   <si>
-    <t>presenting_worthy</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
-    <t>additional_notes</t>
-  </si>
-  <si>
     <t>deprecated, use adorn_totals</t>
   </si>
   <si>
@@ -312,13 +310,85 @@
   </si>
   <si>
     <t>DEPRECATED - says to use dplyr::coalesce() instead</t>
+  </si>
+  <si>
+    <t>additional_notes_sabrina</t>
+  </si>
+  <si>
+    <t>additional_notes_caroline</t>
+  </si>
+  <si>
+    <t>presenting_worthy_first_round</t>
+  </si>
+  <si>
+    <t>presenting_worthy_final</t>
+  </si>
+  <si>
+    <t>look into specifically defining how you want names to be renamed to</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Star Wars Dataverse: Species</t>
+  </si>
+  <si>
+    <t>Kaggle</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/datasets/jsphyg/star-wars</t>
+  </si>
+  <si>
+    <t>Star Wars Dataverse: Films</t>
+  </si>
+  <si>
+    <t>convert to xlsx (make sure dates are in Excel format)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">utilizes average height/lifespan to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> height/lifespan, spongebob meme lettering</t>
+    </r>
+  </si>
+  <si>
+    <t>Star Wars Dataverse: Characters</t>
+  </si>
+  <si>
+    <t>use height for rounding (round_half_up, round_to_fraction, signif_half_up); tabyl's (death status vs BMI); get_dupes(); split into human vs non-human and then use to show compare_df_cols &amp; compare_df_cols_same</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -333,6 +403,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -410,10 +486,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -713,21 +785,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D2BEC45-6A70-274D-AAFF-6DFC31B3AF54}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="44.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="49.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,126 +808,162 @@
         <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="F11" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -864,14 +973,17 @@
       <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>48</v>
+      <c r="D12" t="s">
+        <v>39</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -881,14 +993,17 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>49</v>
+      <c r="D13" t="s">
+        <v>39</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -898,11 +1013,14 @@
       <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -912,42 +1030,51 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>51</v>
+      <c r="D15" t="s">
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>52</v>
+        <v>58</v>
+      </c>
+      <c r="D16" t="s">
+        <v>40</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>53</v>
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -955,16 +1082,19 @@
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>40</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -972,24 +1102,30 @@
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -999,11 +1135,14 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1011,27 +1150,33 @@
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>58</v>
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1041,25 +1186,34 @@
       <c r="C24" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1069,11 +1223,14 @@
       <c r="C26" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1083,33 +1240,42 @@
       <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1119,28 +1285,34 @@
       <c r="C30" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>67</v>
+      <c r="D30" t="s">
+        <v>39</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1148,41 +1320,50 @@
         <v>39</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>69</v>
+        <v>42</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>70</v>
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1190,16 +1371,19 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>72</v>
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
+        <v>40</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1209,11 +1393,14 @@
       <c r="C36" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1221,42 +1408,52 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>75</v>
+        <v>42</v>
+      </c>
+      <c r="D38" t="s">
+        <v>39</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>76</v>
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>40</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <autoFilter ref="D1:D39" xr:uid="{3D2BEC45-6A70-274D-AAFF-6DFC31B3AF54}"/>
+  <conditionalFormatting sqref="C1:D1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"maybe"</formula>
     </cfRule>
@@ -1270,4 +1467,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A38820-6800-4A67-BF45-E3E7F9FE7FDE}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
not really sure what i changed in the excel...
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Biostatistics\Profiles\LinS5\r_code\janitor_function_overview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88687610-5403-4888-9F40-8DF9F52D5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{88687610-5403-4888-9F40-8DF9F52D5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A95545A-4FD4-164F-8B55-03305F236328}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
   <sheets>
     <sheet name="janitor_functions" sheetId="1" r:id="rId1"/>
@@ -388,7 +388,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -410,6 +410,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -428,10 +436,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -440,8 +449,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -791,16 +802,16 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.125" customWidth="1"/>
-    <col min="5" max="5" width="49.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="44.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -820,7 +831,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -834,7 +845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -848,7 +859,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -862,7 +873,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -876,7 +887,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -890,7 +901,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -904,7 +915,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -918,7 +929,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -932,7 +943,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -946,7 +957,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -963,7 +974,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -983,7 +994,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1014,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1020,7 +1031,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1040,7 +1051,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1057,7 +1068,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1085,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1094,7 +1105,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1125,7 +1136,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1142,7 +1153,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1162,7 +1173,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1176,7 +1187,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1196,7 +1207,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1213,7 +1224,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1230,7 +1241,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1247,7 +1258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1261,7 +1272,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1275,7 +1286,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1295,7 +1306,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>64</v>
       </c>
@@ -1312,7 +1323,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1332,7 +1343,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1349,7 +1360,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1363,7 +1374,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1383,7 +1394,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1400,7 +1411,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1417,7 +1428,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1434,7 +1445,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1474,16 +1485,16 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>95</v>
       </c>
@@ -1497,7 +1508,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1507,11 +1518,11 @@
       <c r="C2" t="s">
         <v>104</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -1522,7 +1533,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -1534,6 +1545,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{8677854A-CE94-C34A-8693-466D922F34A7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
still don't know what i changed here
</commit_message>
<xml_diff>
--- a/janitor_functions.xlsx
+++ b/janitor_functions.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{88687610-5403-4888-9F40-8DF9F52D5B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A95545A-4FD4-164F-8B55-03305F236328}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
+    <workbookView xWindow="39160" yWindow="1200" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{19E5A125-1BAE-0E4B-A86F-3AF9B03CEC8B}"/>
   </bookViews>
   <sheets>
     <sheet name="janitor_functions" sheetId="1" r:id="rId1"/>
@@ -497,6 +497,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1484,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A38820-6800-4A67-BF45-E3E7F9FE7FDE}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>